<commit_message>
convert docx to pdf
</commit_message>
<xml_diff>
--- a/server/db/excel/sqlite-inovation-manager-ver-dinh.xlsx
+++ b/server/db/excel/sqlite-inovation-manager-ver-dinh.xlsx
@@ -8,29 +8,30 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DINHNV\MyData\LAPTRINH\NODE4\dinh-inovation\server\db\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7326F623-903F-46CA-AC24-A05775A4EA90}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9727759-77D8-4620-97B4-1C7716D71ACD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="500" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1725" yWindow="1725" windowWidth="19590" windowHeight="10860" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tables" sheetId="1" r:id="rId1"/>
-    <sheet name="parameters" sheetId="13" state="hidden" r:id="rId2"/>
-    <sheet name="admin_menu" sheetId="12" state="hidden" r:id="rId3"/>
-    <sheet name="admin_functions" sheetId="9" state="hidden" r:id="rId4"/>
-    <sheet name="admin_group" sheetId="14" state="hidden" r:id="rId5"/>
-    <sheet name="admin_roles" sheetId="15" state="hidden" r:id="rId6"/>
-    <sheet name="organizations" sheetId="11" state="hidden" r:id="rId7"/>
-    <sheet name="job_roles" sheetId="16" state="hidden" r:id="rId8"/>
-    <sheet name="staffs" sheetId="17" state="hidden" r:id="rId9"/>
-    <sheet name="users" sheetId="10" r:id="rId10"/>
-    <sheet name="ideas_categories" sheetId="19" r:id="rId11"/>
-    <sheet name="ideas_status_type" sheetId="21" r:id="rId12"/>
-    <sheet name="ideas_statuses" sheetId="20" r:id="rId13"/>
-    <sheet name="ideas_questions" sheetId="22" r:id="rId14"/>
+    <sheet name="ideas" sheetId="23" r:id="rId2"/>
+    <sheet name="parameters" sheetId="13" state="hidden" r:id="rId3"/>
+    <sheet name="admin_menu" sheetId="12" state="hidden" r:id="rId4"/>
+    <sheet name="admin_functions" sheetId="9" state="hidden" r:id="rId5"/>
+    <sheet name="admin_group" sheetId="14" state="hidden" r:id="rId6"/>
+    <sheet name="admin_roles" sheetId="15" state="hidden" r:id="rId7"/>
+    <sheet name="organizations" sheetId="11" state="hidden" r:id="rId8"/>
+    <sheet name="job_roles" sheetId="16" state="hidden" r:id="rId9"/>
+    <sheet name="staffs" sheetId="17" state="hidden" r:id="rId10"/>
+    <sheet name="users" sheetId="10" r:id="rId11"/>
+    <sheet name="ideas_categories" sheetId="19" r:id="rId12"/>
+    <sheet name="ideas_status_type" sheetId="21" r:id="rId13"/>
+    <sheet name="ideas_statuses" sheetId="20" r:id="rId14"/>
+    <sheet name="ideas_questions" sheetId="22" r:id="rId15"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">tables!$A$1:$E$52</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">users!$A$1:$N$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">users!$A$1:$N$1</definedName>
   </definedNames>
   <calcPr calcId="145621" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="362">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="705" uniqueCount="377">
   <si>
     <t>table_name</t>
   </si>
@@ -1025,12 +1026,6 @@
     <t>point</t>
   </si>
   <si>
-    <t>ý tưởng nào</t>
-  </si>
-  <si>
-    <t>câu hỏi nào</t>
-  </si>
-  <si>
     <t>cho mấy điểm</t>
   </si>
   <si>
@@ -1118,9 +1113,6 @@
     <t xml:space="preserve">PRIMARY KEY </t>
   </si>
   <si>
-    <t>user nào, (nhớ tạo PRIMARY KEY sau khi tạo đc csdl)</t>
-  </si>
-  <si>
     <t>391 Nguyễn Văn Linh, Đà nẵng</t>
   </si>
   <si>
@@ -1131,6 +1123,93 @@
   </si>
   <si>
     <t>assets/imgs/avatar-dinh.jpg</t>
+  </si>
+  <si>
+    <t>dinh.nguyenvan.ctv</t>
+  </si>
+  <si>
+    <t>nvdinh185</t>
+  </si>
+  <si>
+    <t>assets/imgs/avatar.jpg</t>
+  </si>
+  <si>
+    <t>Ý tưởng này là gì vậy?</t>
+  </si>
+  <si>
+    <t>Mô tả ý tưởng này là gì vậy?</t>
+  </si>
+  <si>
+    <t>Ý tưởng thứ hai là gì vậy?</t>
+  </si>
+  <si>
+    <t>Mô tả ý tưởng thứ hai là gì vậy?</t>
+  </si>
+  <si>
+    <t>Mô tả Ý tưởng của dinh1</t>
+  </si>
+  <si>
+    <t>Ý tưởng thứ hai của dinh1</t>
+  </si>
+  <si>
+    <t>Mô tả Ý tưởng thứ hai của dinh1</t>
+  </si>
+  <si>
+    <t>Ý tưởng đầu tiên của dinh1</t>
+  </si>
+  <si>
+    <t>Ý tưởng đầu tiên của dinh99</t>
+  </si>
+  <si>
+    <t>Mô tả Ý tưởng đầu tiên của dinh99</t>
+  </si>
+  <si>
+    <t>Ý tưởng thứ hai của dinh99</t>
+  </si>
+  <si>
+    <t>Mô tả Ý tưởng thứ hai của dinh99</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">câu hỏi nào </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>(nhớ tạo PRIMARY KEY sau khi tạo đc csdl)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">user nào, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>(nhớ tạo PRIMARY KEY sau khi tạo đc csdl)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ý tưởng nào </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>(tạo PRIMARY KEY khi tạo csdl)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1140,7 +1219,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0;[Red]0"/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1302,6 +1381,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="25">
@@ -1675,7 +1760,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1854,6 +1939,7 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="184">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
@@ -2446,8 +2532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMI74"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B61" sqref="B61"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C69" sqref="C69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="23.25"/>
@@ -3911,10 +3997,10 @@
         <v>18</v>
       </c>
       <c r="B29" s="73" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C29" s="49" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="D29" s="74" t="s">
         <v>322</v>
@@ -4247,10 +4333,10 @@
         <v>262</v>
       </c>
       <c r="B51" s="33" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="C51" s="83" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="D51" s="67" t="s">
         <v>272</v>
@@ -4273,13 +4359,13 @@
     </row>
     <row r="53" spans="1:1023">
       <c r="A53" s="79" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B53" s="31" t="s">
         <v>6</v>
       </c>
       <c r="C53" s="46" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="D53" s="67" t="s">
         <v>272</v>
@@ -5308,13 +5394,13 @@
     </row>
     <row r="54" spans="1:1023">
       <c r="A54" s="79" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B54" s="31" t="s">
         <v>25</v>
       </c>
       <c r="C54" s="46" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="D54" s="67" t="s">
         <v>271</v>
@@ -6341,13 +6427,13 @@
     </row>
     <row r="55" spans="1:1023">
       <c r="A55" s="79" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B55" s="31" t="s">
         <v>2</v>
       </c>
       <c r="C55" s="46" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="D55" s="67" t="s">
         <v>271</v>
@@ -7374,7 +7460,7 @@
     </row>
     <row r="56" spans="1:1023">
       <c r="A56" s="79" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B56" s="31" t="s">
         <v>5</v>
@@ -8407,7 +8493,7 @@
     </row>
     <row r="57" spans="1:1023">
       <c r="A57" s="79" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B57" s="31" t="s">
         <v>11</v>
@@ -9490,10 +9576,10 @@
         <v>265</v>
       </c>
       <c r="B61" s="77" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="C61" s="83" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="D61" s="67" t="s">
         <v>272</v>
@@ -9536,7 +9622,7 @@
         <v>314</v>
       </c>
       <c r="B64" s="73" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C64" s="49" t="s">
         <v>316</v>
@@ -9599,7 +9685,7 @@
         <v>5</v>
       </c>
       <c r="C68" s="49" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="D68" s="70" t="s">
         <v>272</v>
@@ -9613,30 +9699,30 @@
       <c r="B69" s="31" t="s">
         <v>296</v>
       </c>
-      <c r="C69" s="46" t="s">
-        <v>326</v>
+      <c r="C69" s="83" t="s">
+        <v>376</v>
       </c>
       <c r="D69" s="67" t="s">
         <v>272</v>
       </c>
-      <c r="E69" s="5"/>
-    </row>
-    <row r="70" spans="1:5">
+      <c r="E69" s="5" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="38.25">
       <c r="A70" s="55" t="s">
         <v>313</v>
       </c>
       <c r="B70" s="31" t="s">
         <v>317</v>
       </c>
-      <c r="C70" s="46" t="s">
-        <v>327</v>
+      <c r="C70" s="83" t="s">
+        <v>374</v>
       </c>
       <c r="D70" s="67" t="s">
         <v>272</v>
       </c>
-      <c r="E70" s="5" t="s">
-        <v>356</v>
-      </c>
+      <c r="E70" s="5"/>
     </row>
     <row r="71" spans="1:5" ht="38.25">
       <c r="A71" s="55" t="s">
@@ -9645,8 +9731,8 @@
       <c r="B71" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="C71" s="46" t="s">
-        <v>357</v>
+      <c r="C71" s="83" t="s">
+        <v>375</v>
       </c>
       <c r="D71" s="67" t="s">
         <v>272</v>
@@ -9661,7 +9747,7 @@
         <v>325</v>
       </c>
       <c r="C72" s="46" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="D72" s="70" t="s">
         <v>322</v>
@@ -9711,26 +9797,114 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:T1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" ht="18.75">
+      <c r="A1" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="N1" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="P1" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q1" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="R1" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="S1" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="T1" s="16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.140625" customWidth="1"/>
     <col min="4" max="4" width="24.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="33.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="38.28515625" customWidth="1"/>
+    <col min="8" max="8" width="27.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="25.42578125" customWidth="1"/>
     <col min="10" max="10" width="34.42578125" customWidth="1"/>
-    <col min="11" max="11" width="13.7109375" customWidth="1"/>
+    <col min="11" max="11" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="19" style="81" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="19.85546875" style="81" bestFit="1" customWidth="1"/>
   </cols>
@@ -9784,28 +9958,28 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>347</v>
+      </c>
+      <c r="D2" t="s">
+        <v>345</v>
+      </c>
+      <c r="E2" t="s">
+        <v>347</v>
+      </c>
+      <c r="F2" s="78" t="s">
         <v>349</v>
       </c>
-      <c r="D2" t="s">
-        <v>347</v>
-      </c>
-      <c r="E2" t="s">
-        <v>349</v>
-      </c>
-      <c r="F2" s="78" t="s">
-        <v>351</v>
-      </c>
       <c r="G2" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="H2" t="s">
+        <v>355</v>
+      </c>
+      <c r="I2" t="s">
         <v>358</v>
       </c>
-      <c r="I2" t="s">
-        <v>361</v>
-      </c>
       <c r="J2" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="K2">
         <v>1</v>
@@ -9825,28 +9999,28 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="D3" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E3" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F3" s="78" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="G3" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="H3" t="s">
+        <v>355</v>
+      </c>
+      <c r="I3" t="s">
         <v>358</v>
       </c>
-      <c r="I3" t="s">
-        <v>361</v>
-      </c>
       <c r="J3" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="K3">
         <v>99</v>
@@ -9858,6 +10032,47 @@
         <v>1582792430187</v>
       </c>
       <c r="N3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>359</v>
+      </c>
+      <c r="D4" t="s">
+        <v>345</v>
+      </c>
+      <c r="E4" t="s">
+        <v>360</v>
+      </c>
+      <c r="F4" s="78" t="s">
+        <v>349</v>
+      </c>
+      <c r="G4" t="s">
+        <v>346</v>
+      </c>
+      <c r="H4" t="s">
+        <v>355</v>
+      </c>
+      <c r="I4" t="s">
+        <v>361</v>
+      </c>
+      <c r="J4" t="s">
+        <v>331</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4" s="81">
+        <v>1582103204370</v>
+      </c>
+      <c r="M4" s="81">
+        <v>1582792430187</v>
+      </c>
+      <c r="N4">
         <v>1</v>
       </c>
     </row>
@@ -9878,7 +10093,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:E9"/>
   <sheetViews>
@@ -9906,7 +10121,7 @@
         <v>59</v>
       </c>
       <c r="D1" s="37" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="E1" s="37" t="s">
         <v>5</v>
@@ -10045,7 +10260,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:E5"/>
   <sheetViews>
@@ -10086,7 +10301,7 @@
         <v>310</v>
       </c>
       <c r="C2" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="D2">
         <v>4</v>
@@ -10103,7 +10318,7 @@
         <v>282</v>
       </c>
       <c r="C3" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="D3">
         <v>3</v>
@@ -10120,7 +10335,7 @@
         <v>312</v>
       </c>
       <c r="C4" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -10137,7 +10352,7 @@
         <v>311</v>
       </c>
       <c r="C5" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="D5">
         <v>2</v>
@@ -10157,12 +10372,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -10185,7 +10400,7 @@
         <v>25</v>
       </c>
       <c r="D1" s="82" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="E1" s="77" t="s">
         <v>5</v>
@@ -10199,7 +10414,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="5">
@@ -10246,7 +10461,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="5">
@@ -10261,7 +10476,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="5">
@@ -10276,7 +10491,7 @@
         <v>0</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="5">
@@ -10300,7 +10515,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:F6"/>
   <sheetViews>
@@ -10323,7 +10538,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="73" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C1" s="73" t="s">
         <v>318</v>
@@ -10343,7 +10558,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -10363,7 +10578,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -10383,7 +10598,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -10403,7 +10618,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -10423,7 +10638,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -10450,6 +10665,283 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02B7425A-AFAB-46F3-BDD9-8E7F16AA78B9}">
+  <dimension ref="A1:O7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L6" sqref="L6:O7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" style="81" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" ht="18.75">
+      <c r="A1" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="31" t="s">
+        <v>248</v>
+      </c>
+      <c r="E1" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="84" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="33" t="s">
+        <v>285</v>
+      </c>
+      <c r="I1" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" s="31" t="s">
+        <v>297</v>
+      </c>
+      <c r="L1" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" s="31" t="s">
+        <v>260</v>
+      </c>
+      <c r="N1" s="73" t="s">
+        <v>328</v>
+      </c>
+      <c r="O1" s="76" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>362</v>
+      </c>
+      <c r="C2" t="s">
+        <v>363</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>3</v>
+      </c>
+      <c r="G2" s="81">
+        <v>1590045283916</v>
+      </c>
+      <c r="H2" t="s">
+        <v>359</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>364</v>
+      </c>
+      <c r="C3" t="s">
+        <v>365</v>
+      </c>
+      <c r="E3">
+        <v>5</v>
+      </c>
+      <c r="F3">
+        <v>3</v>
+      </c>
+      <c r="G3" s="81">
+        <v>1590045323073</v>
+      </c>
+      <c r="H3" t="s">
+        <v>359</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>369</v>
+      </c>
+      <c r="C4" t="s">
+        <v>366</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" s="81">
+        <v>1590045603862</v>
+      </c>
+      <c r="H4" t="s">
+        <v>347</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>367</v>
+      </c>
+      <c r="C5" t="s">
+        <v>368</v>
+      </c>
+      <c r="E5">
+        <v>7</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5" s="81">
+        <v>1590045634319</v>
+      </c>
+      <c r="H5" t="s">
+        <v>347</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>370</v>
+      </c>
+      <c r="C6" t="s">
+        <v>371</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+      <c r="G6" s="81">
+        <v>1590047016939</v>
+      </c>
+      <c r="H6" t="s">
+        <v>348</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>372</v>
+      </c>
+      <c r="C7" t="s">
+        <v>373</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+      <c r="G7" s="81">
+        <v>1590047072983</v>
+      </c>
+      <c r="H7" t="s">
+        <v>348</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L1"/>
   <sheetViews>
@@ -10521,7 +11013,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Q1"/>
   <sheetViews>
@@ -10594,7 +11086,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I53"/>
   <sheetViews>
@@ -11539,7 +12031,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:H1"/>
   <sheetViews>
@@ -11595,7 +12087,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:I1"/>
   <sheetViews>
@@ -11655,7 +12147,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:R3"/>
   <sheetViews>
@@ -11780,7 +12272,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:R1"/>
   <sheetViews>
@@ -11874,92 +12366,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:T1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:20" ht="18.75">
-      <c r="A1" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="I1" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="K1" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="L1" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="M1" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="N1" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="O1" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="P1" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q1" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="R1" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="S1" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="T1" s="16" t="s">
-        <v>11</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
edit client and server
</commit_message>
<xml_diff>
--- a/server/db/excel/sqlite-inovation-manager-ver-dinh.xlsx
+++ b/server/db/excel/sqlite-inovation-manager-ver-dinh.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DINHNV\MyData\LAPTRINH\NODE4\dinh-inovation\server\db\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9727759-77D8-4620-97B4-1C7716D71ACD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF918709-1420-4A0C-8D56-47068757686C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1725" yWindow="1725" windowWidth="19590" windowHeight="10860" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="500" firstSheet="1" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tables" sheetId="1" r:id="rId1"/>
@@ -1146,9 +1146,6 @@
     <t>Mô tả ý tưởng thứ hai là gì vậy?</t>
   </si>
   <si>
-    <t>Mô tả Ý tưởng của dinh1</t>
-  </si>
-  <si>
     <t>Ý tưởng thứ hai của dinh1</t>
   </si>
   <si>
@@ -1210,6 +1207,9 @@
       </rPr>
       <t>(tạo PRIMARY KEY khi tạo csdl)</t>
     </r>
+  </si>
+  <si>
+    <t>Mô tả Ý tưởng đầu tiên của dinh1</t>
   </si>
 </sst>
 </file>
@@ -2532,8 +2532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMI74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C69" sqref="C69"/>
+    <sheetView topLeftCell="A58" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="23.25"/>
@@ -9700,7 +9700,7 @@
         <v>296</v>
       </c>
       <c r="C69" s="83" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D69" s="67" t="s">
         <v>272</v>
@@ -9717,7 +9717,7 @@
         <v>317</v>
       </c>
       <c r="C70" s="83" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D70" s="67" t="s">
         <v>272</v>
@@ -9732,7 +9732,7 @@
         <v>13</v>
       </c>
       <c r="C71" s="83" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D71" s="67" t="s">
         <v>272</v>
@@ -10098,7 +10098,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -10377,7 +10377,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -10495,7 +10495,7 @@
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="5">
-        <v>995</v>
+        <v>999</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -10519,8 +10519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -10669,13 +10669,16 @@
   <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L6" sqref="L6:O7"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.7109375" style="81" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="18.75">
@@ -10800,10 +10803,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C4" t="s">
-        <v>366</v>
+        <v>376</v>
       </c>
       <c r="E4">
         <v>3</v>
@@ -10835,10 +10838,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>366</v>
+      </c>
+      <c r="C5" t="s">
         <v>367</v>
-      </c>
-      <c r="C5" t="s">
-        <v>368</v>
       </c>
       <c r="E5">
         <v>7</v>
@@ -10870,13 +10873,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>369</v>
+      </c>
+      <c r="C6" t="s">
         <v>370</v>
       </c>
-      <c r="C6" t="s">
-        <v>371</v>
-      </c>
       <c r="E6">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F6">
         <v>2</v>
@@ -10905,10 +10908,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>371</v>
+      </c>
+      <c r="C7" t="s">
         <v>372</v>
-      </c>
-      <c r="C7" t="s">
-        <v>373</v>
       </c>
       <c r="E7">
         <v>2</v>

</xml_diff>